<commit_message>
Updated the function names and logging features
</commit_message>
<xml_diff>
--- a/sotcddatabasetests/executioninfo/input-data/SuiteA.xlsx
+++ b/sotcddatabasetests/executioninfo/input-data/SuiteA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>TestA1</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>getAssets</t>
-  </si>
-  <si>
     <t>OpendbConnection</t>
   </si>
   <si>
@@ -93,12 +87,6 @@
     <t>query</t>
   </si>
   <si>
-    <t>TestA2</t>
-  </si>
-  <si>
-    <t>TestA4</t>
-  </si>
-  <si>
     <t>select count(*) from tbl_assets</t>
   </si>
   <si>
@@ -114,9 +102,6 @@
     <t>select count(*) from tbl_sharelink</t>
   </si>
   <si>
-    <t>ActiveShowsTest</t>
-  </si>
-  <si>
     <t>select count(*) from tbl_sharelink where playname&lt;&gt;''</t>
   </si>
   <si>
@@ -126,7 +111,28 @@
     <t>4</t>
   </si>
   <si>
-    <t>getShows</t>
+    <t>getActiveShowsCount</t>
+  </si>
+  <si>
+    <t>getActiveShowsNames</t>
+  </si>
+  <si>
+    <t>ActiveShowsCountTest</t>
+  </si>
+  <si>
+    <t>ActiveShowsListTest</t>
+  </si>
+  <si>
+    <t>SetUpDbConnection</t>
+  </si>
+  <si>
+    <t>CloseDbConnection</t>
+  </si>
+  <si>
+    <t>GetAsset_Shows_Users_Count</t>
+  </si>
+  <si>
+    <t>getRecordCount</t>
   </si>
 </sst>
 </file>
@@ -535,7 +541,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -557,34 +563,42 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>26</v>
+      <c r="A5" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -594,15 +608,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="20.7265625" customWidth="1"/>
     <col min="2" max="2" width="17.1796875" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="35.90625" style="10" customWidth="1"/>
@@ -612,43 +626,43 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6" t="s">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>35</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="6" t="s">
-        <v>25</v>
+      <c r="A3" t="s">
+        <v>37</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="6"/>
@@ -656,11 +670,11 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="6"/>
@@ -668,15 +682,27 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -686,10 +712,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -707,162 +733,194 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" t="s">
         <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to get assets for a show
</commit_message>
<xml_diff>
--- a/sotcddatabasetests/executioninfo/input-data/SuiteA.xlsx
+++ b/sotcddatabasetests/executioninfo/input-data/SuiteA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -72,9 +72,6 @@
     <t>postgres</t>
   </si>
   <si>
-    <t>senthilrun</t>
-  </si>
-  <si>
     <t>10.37.4.140:5432</t>
   </si>
   <si>
@@ -133,6 +130,24 @@
   </si>
   <si>
     <t>getRecordCount</t>
+  </si>
+  <si>
+    <t>getAssetsinShow</t>
+  </si>
+  <si>
+    <t>showname</t>
+  </si>
+  <si>
+    <t>GetAssetsinShowTest</t>
+  </si>
+  <si>
+    <t>Photoshoot</t>
+  </si>
+  <si>
+    <t>vidhya</t>
+  </si>
+  <si>
+    <t>Buffalo Photos</t>
   </si>
 </sst>
 </file>
@@ -220,7 +235,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -244,6 +259,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -541,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -563,7 +583,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -571,7 +591,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -579,7 +599,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -587,17 +607,25 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>36</v>
+      <c r="A6" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -608,10 +636,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -646,7 +674,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" t="s">
@@ -658,11 +686,11 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="6"/>
@@ -670,11 +698,11 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="6"/>
@@ -682,27 +710,38 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>36</v>
+      <c r="A6" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -712,10 +751,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -733,7 +772,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -756,7 +795,7 @@
         <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -767,7 +806,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -776,15 +815,15 @@
         <v>17</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -795,7 +834,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -806,45 +845,45 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -855,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -866,12 +905,12 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -882,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -893,7 +932,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -901,7 +940,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -912,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -920,6 +959,44 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the changes for View Assets by ShowNames
</commit_message>
<xml_diff>
--- a/sotcddatabasetests/executioninfo/input-data/SuiteA.xlsx
+++ b/sotcddatabasetests/executioninfo/input-data/SuiteA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Buffalo Photos</t>
+  </si>
+  <si>
+    <t>Jasper</t>
   </si>
 </sst>
 </file>
@@ -751,10 +754,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -962,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -973,30 +976,41 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="4" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>